<commit_message>
Bitmap save to file
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="51">
   <si>
     <t>biSize</t>
   </si>
@@ -137,9 +137,6 @@
     <t>BITMAPCOREHEADER</t>
   </si>
   <si>
-    <t>(OS2)</t>
-  </si>
-  <si>
     <t>(without CSType)</t>
   </si>
   <si>
@@ -162,6 +159,24 @@
   </si>
   <si>
     <t>V3(,5)</t>
+  </si>
+  <si>
+    <t>(OS/2)</t>
+  </si>
+  <si>
+    <t>=12</t>
+  </si>
+  <si>
+    <t>=40</t>
+  </si>
+  <si>
+    <t>=56</t>
+  </si>
+  <si>
+    <t>=108</t>
+  </si>
+  <si>
+    <t>=124</t>
   </si>
 </sst>
 </file>
@@ -205,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -213,16 +228,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -503,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF36"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +630,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -564,7 +650,7 @@
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -606,7 +692,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -645,7 +731,9 @@
         <f>IF(C3="", "", IF(C3="Long", 4, IF(C3="Integer", 2, 0)))</f>
         <v>4</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
@@ -662,7 +750,9 @@
         <f>IF(I3="", "", IF(I3="Long", 4, IF(I3="Integer", 2, 0)))</f>
         <v>4</v>
       </c>
-      <c r="L3" s="3"/>
+      <c r="L3" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="M3" s="3" t="str">
         <f>A3</f>
         <v>biSize</v>
@@ -680,7 +770,9 @@
         <f>IF(O3="", "", IF(O3="Long", 4, IF(O3="Integer", 2, 0)))</f>
         <v>4</v>
       </c>
-      <c r="R3" s="3"/>
+      <c r="R3" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="S3" s="3" t="str">
         <f>G3</f>
         <v>biSize</v>
@@ -698,7 +790,9 @@
         <f>IF(U3="", "", IF(U3="Long", 4, IF(U3="Integer", 2, 0)))</f>
         <v>4</v>
       </c>
-      <c r="X3" s="3"/>
+      <c r="X3" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="Y3" s="3" t="str">
         <f>S3</f>
         <v>biSize</v>
@@ -715,7 +809,9 @@
       <c r="AC3" s="3">
         <v>4</v>
       </c>
-      <c r="AD3" s="3"/>
+      <c r="AD3" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
     </row>
@@ -768,7 +864,7 @@
         <v>3</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" ref="Q4:Q21" si="2">IF(O4="", "", IF(O4="Long", 4, IF(O4="Integer", 2, 0)))</f>
+        <f t="shared" ref="Q4" si="2">IF(O4="", "", IF(O4="Long", 4, IF(O4="Integer", 2, 0)))</f>
         <v>4</v>
       </c>
       <c r="R4" s="3"/>
@@ -856,19 +952,19 @@
       <c r="AF5" s="3"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
@@ -904,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="Q6" s="3">
-        <f t="shared" ref="Q6:Q21" si="5">IF(O6="", "", IF(O6="Long", 4, IF(O6="Integer", 2, 0)))</f>
+        <f t="shared" ref="Q6:Q16" si="5">IF(O6="", "", IF(O6="Long", 4, IF(O6="Integer", 2, 0)))</f>
         <v>4</v>
       </c>
       <c r="R6" s="3"/>
@@ -947,19 +1043,19 @@
       <c r="AF6" s="3"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="D7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="12">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
@@ -1010,73 +1106,73 @@
         <v>12</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="H8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="J8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L8" s="3"/>
-      <c r="M8" s="3" t="str">
+      <c r="M8" s="5" t="str">
         <f>G8</f>
         <v>biPlanes</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="N8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="P8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="10">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="R8" s="3"/>
-      <c r="S8" s="3" t="str">
+      <c r="S8" s="5" t="str">
         <f>G8</f>
         <v>biPlanes</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="1" t="s">
+      <c r="T8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="V8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W8" s="3">
+      <c r="V8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="W8" s="10">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="X8" s="3"/>
-      <c r="Y8" s="3" t="str">
+      <c r="Y8" s="5" t="str">
         <f>S8</f>
         <v>biPlanes</v>
       </c>
-      <c r="Z8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="1" t="s">
+      <c r="Z8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AB8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC8" s="3">
+      <c r="AB8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC8" s="10">
         <v>2</v>
       </c>
       <c r="AD8" s="3"/>
@@ -1085,80 +1181,80 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="H9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="J9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L9" s="3"/>
-      <c r="M9" s="3" t="str">
-        <f t="shared" ref="M9:M17" si="6">G9</f>
+      <c r="M9" s="7" t="str">
+        <f t="shared" ref="M9:M16" si="6">G9</f>
         <v>biBitCount</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="1" t="s">
+      <c r="N9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="3">
+      <c r="P9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="12">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="R9" s="3"/>
-      <c r="S9" s="3" t="str">
+      <c r="S9" s="7" t="str">
         <f>G9</f>
         <v>biBitCount</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U9" s="1" t="s">
+      <c r="T9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="V9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W9" s="3">
+      <c r="V9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9" s="12">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="X9" s="3"/>
-      <c r="Y9" s="3" t="str">
+      <c r="Y9" s="7" t="str">
         <f>S9</f>
         <v>biBitCount</v>
       </c>
-      <c r="Z9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="1" t="s">
+      <c r="Z9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AB9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC9" s="3">
+      <c r="AB9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="12">
         <v>2</v>
       </c>
       <c r="AD9" s="3"/>
@@ -1167,7 +1263,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1743,7 +1839,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1812,7 +1908,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -2029,40 +2125,6 @@
         <v>56</v>
       </c>
       <c r="R22" s="3"/>
-      <c r="S22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W22" s="3">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>bV4CSType</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC22" s="3">
-        <v>4</v>
-      </c>
-      <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
     </row>
@@ -2085,17 +2147,39 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
+      <c r="S23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W23" s="3">
+        <f>IF(U23="", "", IF(U23="Long", 4, IF(U23="Integer", 2, 0)))</f>
+        <v>4</v>
+      </c>
       <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
+      <c r="Y23" s="3" t="str">
+        <f>S23</f>
+        <v>bV4CSType</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>4</v>
+      </c>
       <c r="AD23" s="3"/>
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
@@ -2114,45 +2198,24 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
-      <c r="S24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W24" s="3">
-        <v>36</v>
-      </c>
+      <c r="S24" s="3"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>bV4Endpoints</v>
-      </c>
-      <c r="Z24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC24" s="3">
-        <v>36</v>
-      </c>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
@@ -2176,17 +2239,38 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
+      <c r="S25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W25" s="3">
+        <v>36</v>
+      </c>
       <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="3"/>
+      <c r="Y25" s="3" t="str">
+        <f>S25</f>
+        <v>bV4Endpoints</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>36</v>
+      </c>
       <c r="AD25" s="3"/>
       <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
@@ -2210,38 +2294,17 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
-      <c r="S26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W26" s="3">
-        <v>4</v>
-      </c>
+      <c r="S26" s="3"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="Y26" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>bV4GammaRed</v>
-      </c>
-      <c r="Z26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC26" s="3">
-        <v>4</v>
-      </c>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
@@ -2266,7 +2329,7 @@
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T27" s="1" t="s">
         <v>1</v>
@@ -2282,8 +2345,8 @@
       </c>
       <c r="X27" s="3"/>
       <c r="Y27" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>bV4GammaGreen</v>
+        <f>S27</f>
+        <v>bV4GammaRed</v>
       </c>
       <c r="Z27" s="1" t="s">
         <v>1</v>
@@ -2321,7 +2384,7 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T28" s="1" t="s">
         <v>1</v>
@@ -2337,8 +2400,8 @@
       </c>
       <c r="X28" s="3"/>
       <c r="Y28" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>bV4GammaBlue</v>
+        <f>S28</f>
+        <v>bV4GammaGreen</v>
       </c>
       <c r="Z28" s="1" t="s">
         <v>1</v>
@@ -2375,20 +2438,38 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
+      <c r="S29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V29" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="W29" s="3">
-        <f>SUM(W3:W28)</f>
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="3"/>
+      <c r="Y29" s="3" t="str">
+        <f>S29</f>
+        <v>bV4GammaBlue</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>4</v>
+      </c>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
@@ -2412,29 +2493,20 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="S30" s="3"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
+      <c r="W30" s="3">
+        <f>SUM(W3:W29)</f>
+        <v>108</v>
+      </c>
       <c r="X30" s="3"/>
-      <c r="Y30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC30" s="3">
-        <v>4</v>
-      </c>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
@@ -2458,14 +2530,16 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
+      <c r="S31" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z31" s="1" t="s">
         <v>1</v>
@@ -2509,7 +2583,7 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Z32" s="1" t="s">
         <v>1</v>
@@ -2553,7 +2627,7 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
       <c r="Y33" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Z33" s="1" t="s">
         <v>1</v>
@@ -2596,13 +2670,20 @@
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
+      <c r="Y34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB34" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AC34" s="3">
-        <f>SUM(AC3:AC33)</f>
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
@@ -2633,13 +2714,14 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
-      <c r="AC35" s="3"/>
+      <c r="AC35" s="3">
+        <f>SUM(AC3:AC34)</f>
+        <v>124</v>
+      </c>
       <c r="AD35" s="3"/>
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
@@ -2663,20 +2745,36 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="2"/>
-      <c r="AD36" s="2"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>